<commit_message>
updating data template style and adding lifestage
</commit_message>
<xml_diff>
--- a/inst/template/template-data.xlsx
+++ b/inst/template/template-data.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <si>
     <t xml:space="preserve">latin_name</t>
   </si>
@@ -28,6 +25,9 @@
     <t xml:space="preserve">effect</t>
   </si>
   <si>
+    <t xml:space="preserve">lifestage</t>
+  </si>
+  <si>
     <t xml:space="preserve">simple_lifestage</t>
   </si>
   <si>
@@ -46,33 +46,18 @@
     <t xml:space="preserve">species_present_in_bc</t>
   </si>
   <si>
+    <t xml:space="preserve">column_name</t>
+  </si>
+  <si>
     <t xml:space="preserve">description</t>
   </si>
   <si>
+    <t xml:space="preserve">allowed_values</t>
+  </si>
+  <si>
     <t xml:space="preserve">example</t>
   </si>
   <si>
-    <t xml:space="preserve">chk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c("")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c(0, 9000000)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c(0, 40000)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pkey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">column_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allowed_values</t>
-  </si>
-  <si>
     <t xml:space="preserve">extra_details</t>
   </si>
   <si>
@@ -106,10 +91,19 @@
     <t xml:space="preserve">The lifestage of the species during the test.</t>
   </si>
   <si>
+    <t xml:space="preserve">Any lifestage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">egg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A simplified lifestage that is based on the lifestage.</t>
+  </si>
+  <si>
     <t xml:space="preserve">One of els, adult, or juvenile</t>
   </si>
   <si>
-    <t xml:space="preserve">juvenile</t>
+    <t xml:space="preserve">els</t>
   </si>
   <si>
     <t xml:space="preserve">early life stage (els)</t>
@@ -887,80 +881,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -977,157 +897,172 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>32</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6"/>
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10"/>
+      <c r="E11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1145,498 +1080,498 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B36" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B37" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B38" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B39" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B40" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B41" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B43" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B44" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B45" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B46" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B47" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B48" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B49" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B50" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B51" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B52" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B53" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B54" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B55" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B56" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B57" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B58" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B59" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B60" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B61" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>